<commit_message>
Work on real student grouping data example
</commit_message>
<xml_diff>
--- a/src/samples/students_excel/Groups.xlsx
+++ b/src/samples/students_excel/Groups.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\h\Development\FYP\final-year-project\src\samples\students_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6297F929-6C20-48CE-B8F1-2ECEE24715E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01D8A85A-48A1-4770-8F74-EC183533A45B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{611A7E27-F5CC-449F-B454-7FBE7711AE83}"/>
   </bookViews>
@@ -1559,8 +1559,8 @@
   <dimension ref="A1:H312"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A109" sqref="A109:H312"/>
+      <pane ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G108" sqref="G108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>

</xml_diff>